<commit_message>
added heat recycling for lime and o2
</commit_message>
<xml_diff>
--- a/data/steel/steel_factories.xlsx
+++ b/data/steel/steel_factories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49A5E71-5C0D-2245-848C-857B5A095DEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C45699C-A996-FB43-9108-5414A51DECA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="460" windowWidth="26520" windowHeight="16520" activeTab="1" xr2:uid="{67EB8BFD-A7DA-B046-8505-BD4010EFF077}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="57">
   <si>
     <t>Inflow</t>
   </si>
@@ -101,16 +101,10 @@
     <t>outflow</t>
   </si>
   <si>
-    <t>aux_lime_kiln</t>
-  </si>
-  <si>
     <t>O2</t>
   </si>
   <si>
     <t>O2__pure</t>
-  </si>
-  <si>
-    <t>aux_air_seperation</t>
   </si>
   <si>
     <t>oxygen</t>
@@ -595,7 +589,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,19 +601,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -633,21 +627,21 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -661,49 +655,49 @@
         <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -716,7 +710,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -746,10 +740,10 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s">
         <v>18</v>
@@ -778,25 +772,25 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
         <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -804,7 +798,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -818,8 +812,8 @@
       <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
-        <v>24</v>
+      <c r="H3" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="I3" t="s">
         <v>13</v>
@@ -830,25 +824,25 @@
         <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -856,25 +850,25 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" t="s">
         <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -882,103 +876,103 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
         <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" t="s">
         <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" t="s">
         <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -986,25 +980,25 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1012,258 +1006,258 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="I17" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>24</v>
+      <c r="H18" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1302,7 +1296,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
@@ -1313,7 +1307,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
@@ -1324,7 +1318,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>6</v>
@@ -1335,7 +1329,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -1346,7 +1340,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>

</xml_diff>